<commit_message>
added secondary ID column
</commit_message>
<xml_diff>
--- a/emx/dist/rd3_portal_novelomics.xlsx
+++ b/emx/dist/rd3_portal_novelomics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="79">
   <si>
     <t>rd3_portal</t>
   </si>
@@ -33,7 +33,7 @@
     <t>RD3 portal, containing data submitted by CNAG</t>
   </si>
   <si>
-    <t>Staging tables for novel omics sample and experiment metadata (v1.0.0, 2021-09-20)</t>
+    <t>Staging tables for novel omics sample and experiment metadata (v1.1.0, 2021-09-28)</t>
   </si>
   <si>
     <t>experiment</t>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>ERN</t>
+  </si>
+  <si>
+    <t>CNAG_barcode</t>
   </si>
   <si>
     <t>string</t>
@@ -604,16 +607,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -656,16 +659,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -703,7 +706,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -711,25 +714,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -743,7 +746,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -763,7 +766,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -783,7 +786,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -803,7 +806,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -823,7 +826,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -843,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -863,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -883,7 +886,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -903,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -923,7 +926,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -943,7 +946,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -963,7 +966,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -983,7 +986,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -1003,7 +1006,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -1023,7 +1026,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -1043,7 +1046,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -1063,7 +1066,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -1083,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -1103,7 +1106,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
@@ -1123,7 +1126,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -1143,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -1163,7 +1166,7 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -1183,7 +1186,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -1203,7 +1206,7 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
@@ -1223,7 +1226,7 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -1243,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -1263,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -1283,7 +1286,7 @@
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -1303,7 +1306,7 @@
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
@@ -1323,7 +1326,7 @@
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>
@@ -1343,7 +1346,7 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
@@ -1363,7 +1366,7 @@
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -1383,7 +1386,7 @@
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -1403,7 +1406,7 @@
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
@@ -1423,7 +1426,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -1443,7 +1446,7 @@
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -1463,7 +1466,7 @@
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
@@ -1483,7 +1486,7 @@
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
@@ -1503,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E40" t="b">
         <v>0</v>
@@ -1523,7 +1526,7 @@
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E41" t="b">
         <v>0</v>
@@ -1543,7 +1546,7 @@
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
@@ -1563,7 +1566,7 @@
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -1583,7 +1586,7 @@
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
@@ -1603,7 +1606,7 @@
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E45" t="b">
         <v>0</v>
@@ -1626,7 +1629,7 @@
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E46" t="b">
         <v>1</v>
@@ -1646,7 +1649,7 @@
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
@@ -1666,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
@@ -1686,7 +1689,7 @@
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -1706,7 +1709,7 @@
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
@@ -1726,7 +1729,7 @@
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
@@ -1746,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E52" t="b">
         <v>0</v>
@@ -1766,7 +1769,7 @@
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E53" t="b">
         <v>0</v>
@@ -1786,7 +1789,7 @@
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E54" t="b">
         <v>0</v>
@@ -1806,7 +1809,7 @@
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E55" t="b">
         <v>0</v>
@@ -1820,7 +1823,7 @@
         <v>13</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
@@ -1833,9 +1836,6 @@
       </c>
       <c r="F56" t="b">
         <v>1</v>
-      </c>
-      <c r="G56" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1843,18 +1843,41 @@
         <v>13</v>
       </c>
       <c r="B57" t="s">
+        <v>57</v>
+      </c>
+      <c r="C57" t="b">
+        <v>0</v>
+      </c>
+      <c r="D57" t="s">
+        <v>67</v>
+      </c>
+      <c r="E57" t="b">
+        <v>0</v>
+      </c>
+      <c r="F57" t="b">
+        <v>1</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" t="s">
         <v>58</v>
       </c>
-      <c r="C57" t="b">
-        <v>1</v>
-      </c>
-      <c r="D57" t="s">
-        <v>65</v>
-      </c>
-      <c r="E57" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" t="b">
+      <c r="C58" t="b">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>66</v>
+      </c>
+      <c r="E58" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added dataCreated attribute and rebuilt EMX
</commit_message>
<xml_diff>
--- a/emx/dist/rd3_portal_novelomics.xlsx
+++ b/emx/dist/rd3_portal_novelomics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="81">
   <si>
     <t>rd3_portal</t>
   </si>
@@ -33,7 +33,7 @@
     <t>RD3 portal, containing data submitted by CNAG</t>
   </si>
   <si>
-    <t>Staging tables for novel omics sample and experiment metadata (v1.1.0, 2021-09-28)</t>
+    <t>Staging tables for novel omics sample and experiment metadata (v1.3.0, 2021-10-11)</t>
   </si>
   <si>
     <t>experiment</t>
@@ -189,6 +189,9 @@
     <t>sample_ega_id</t>
   </si>
   <si>
+    <t>date_created</t>
+  </si>
+  <si>
     <t>processed</t>
   </si>
   <si>
@@ -220,6 +223,9 @@
   </si>
   <si>
     <t>bool</t>
+  </si>
+  <si>
+    <t>Date the data was uploaded into RD3</t>
   </si>
   <si>
     <t>name</t>
@@ -607,16 +613,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -659,16 +665,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -706,36 +712,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>72</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -746,7 +755,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -755,7 +764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -766,7 +775,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -775,7 +784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -786,7 +795,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -795,7 +804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -806,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -815,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -826,7 +835,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -835,7 +844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -846,7 +855,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -855,7 +864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -866,7 +875,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -875,7 +884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -886,7 +895,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -895,7 +904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -906,7 +915,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -915,7 +924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -926,7 +935,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -935,7 +944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -946,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -955,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -966,7 +975,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -975,7 +984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -986,7 +995,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -995,7 +1004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1006,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -1015,7 +1024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1026,7 +1035,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -1046,7 +1055,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -1066,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -1086,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -1106,7 +1115,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
@@ -1126,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -1146,7 +1155,7 @@
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -1166,7 +1175,7 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -1186,7 +1195,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -1206,7 +1215,7 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
@@ -1226,7 +1235,7 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -1246,7 +1255,7 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -1266,7 +1275,7 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -1286,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -1306,7 +1315,7 @@
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
@@ -1326,7 +1335,7 @@
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>
@@ -1346,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
@@ -1355,7 +1364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -1366,7 +1375,7 @@
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -1375,7 +1384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1386,7 +1395,7 @@
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -1395,7 +1404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -1406,7 +1415,7 @@
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
@@ -1415,7 +1424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -1426,7 +1435,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -1435,7 +1444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -1446,7 +1455,7 @@
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -1455,7 +1464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -1466,7 +1475,7 @@
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
@@ -1475,7 +1484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -1486,7 +1495,7 @@
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
@@ -1495,7 +1504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -1506,7 +1515,7 @@
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E40" t="b">
         <v>0</v>
@@ -1515,7 +1524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -1526,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E41" t="b">
         <v>0</v>
@@ -1535,7 +1544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -1546,7 +1555,7 @@
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
@@ -1555,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -1566,7 +1575,7 @@
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -1575,7 +1584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -1586,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
@@ -1595,7 +1604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -1614,11 +1623,11 @@
       <c r="F45" t="b">
         <v>1</v>
       </c>
-      <c r="G45" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="G45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -1626,50 +1635,53 @@
         <v>58</v>
       </c>
       <c r="C46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="C47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>13</v>
       </c>
       <c r="B48" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
@@ -1678,7 +1690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -1689,7 +1701,7 @@
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -1698,18 +1710,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
@@ -1718,18 +1730,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
@@ -1738,18 +1750,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E52" t="b">
         <v>0</v>
@@ -1758,7 +1770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -1769,7 +1781,7 @@
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E53" t="b">
         <v>0</v>
@@ -1778,7 +1790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>13</v>
       </c>
@@ -1789,7 +1801,7 @@
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E54" t="b">
         <v>0</v>
@@ -1798,7 +1810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -1809,7 +1821,7 @@
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E55" t="b">
         <v>0</v>
@@ -1818,7 +1830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>13</v>
       </c>
@@ -1829,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E56" t="b">
         <v>0</v>
@@ -1838,12 +1850,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>13</v>
       </c>
       <c r="B57" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C57" t="b">
         <v>0</v>
@@ -1857,27 +1869,70 @@
       <c r="F57" t="b">
         <v>1</v>
       </c>
-      <c r="G57" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>13</v>
       </c>
       <c r="B58" t="s">
+        <v>57</v>
+      </c>
+      <c r="C58" t="b">
+        <v>0</v>
+      </c>
+      <c r="D58" t="s">
+        <v>67</v>
+      </c>
+      <c r="E58" t="b">
+        <v>0</v>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+      <c r="G58" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" t="s">
         <v>58</v>
       </c>
-      <c r="C58" t="b">
-        <v>1</v>
-      </c>
-      <c r="D58" t="s">
-        <v>66</v>
-      </c>
-      <c r="E58" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" t="b">
+      <c r="C59" t="b">
+        <v>0</v>
+      </c>
+      <c r="D59" t="s">
+        <v>68</v>
+      </c>
+      <c r="E59" t="b">
+        <v>0</v>
+      </c>
+      <c r="F59" t="b">
+        <v>1</v>
+      </c>
+      <c r="H59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60" t="b">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
+        <v>67</v>
+      </c>
+      <c r="E60" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed portal date attribute
</commit_message>
<xml_diff>
--- a/emx/dist/rd3_portal_novelomics.xlsx
+++ b/emx/dist/rd3_portal_novelomics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="82">
   <si>
     <t>rd3_portal</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>datetime</t>
   </si>
   <si>
     <t>bool</t>
@@ -613,16 +616,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -665,16 +668,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -720,28 +723,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1612,10 +1615,10 @@
         <v>57</v>
       </c>
       <c r="C45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E45" t="b">
         <v>0</v>
@@ -1624,7 +1627,7 @@
         <v>1</v>
       </c>
       <c r="G45" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1638,7 +1641,7 @@
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
@@ -1878,10 +1881,10 @@
         <v>57</v>
       </c>
       <c r="C58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E58" t="b">
         <v>0</v>
@@ -1890,7 +1893,7 @@
         <v>1</v>
       </c>
       <c r="G58" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1904,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E59" t="b">
         <v>0</v>

</xml_diff>